<commit_message>
PDF Content extraction working, but without spacing on words
</commit_message>
<xml_diff>
--- a/Jim_OICRs_URLs.xlsx
+++ b/Jim_OICRs_URLs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLBKMVE\urls-content-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F05F39-5AD6-4F00-BEDD-B31234C45A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF2B14F-6342-461A-B9A4-1D692241F2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18240" yWindow="4580" windowWidth="18360" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17900" yWindow="4240" windowWidth="18360" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,17 +23,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="新細明體, sans-serif"/>
-      </rPr>
-      <t>https://marlo.cgiar.org/projects/Livestock/studySummary.do?studyID=3560&amp;cycle=Reporting&amp;year=2021</t>
-    </r>
   </si>
   <si>
     <r>
@@ -57,12 +46,15 @@
       <t>https://marlo.cgiar.org/projects/CCAFS/studySummary.do?studyID=2600&amp;cycle=Reporting&amp;year=2018, https://marlo.cgiar.org/projects/CCAFS/studySummary.do?studyID=2362&amp;cycle=Reporting&amp;year=2019, https://marlo.cgiar.org/projects/CCAFS/studySummary.do?studyID=3790&amp;cycle=Reporting&amp;year=2020</t>
     </r>
   </si>
+  <si>
+    <t>https://hdl.handle.net/10568/121501</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -98,6 +90,13 @@
       <sz val="12"/>
       <color rgb="FF1155CC"/>
       <name val="Helvetica, sans-serif"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,16 +116,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -346,7 +348,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -357,18 +359,18 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>